<commit_message>
MCB rates integration done
</commit_message>
<xml_diff>
--- a/docs/exchange_rates.xlsx
+++ b/docs/exchange_rates.xlsx
@@ -1038,7 +1038,7 @@
     </x:row>
     <x:row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <x:c r="A3" s="1" t="str">
-        <x:v>INDICATIVE FOREIGN EXCHANGE RATES AS AT 04-Jan-2025</x:v>
+        <x:v>INDICATIVE FOREIGN EXCHANGE RATES AS AT 07-Feb-2025</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1115,6 +1115,811 @@
       <x:c r="K9" s="8"/>
     </x:row>
     <x:row r="9"/>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>AUSTRALIA</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Australia Dollars</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>AUD</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>29.36</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>29.01</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>30.8</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>30.8</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>CANADA</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Canadian Dollar</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>CAD</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>32.75</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>32.65</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>32.26</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>34.35</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>34.35</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>34.35</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>CHINA</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>China Yuan Renminbi</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>CNY</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>6.36</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>6.69</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>EUR COUNTRIES</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Euro</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>EUR</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>47.83</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>47.71</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>47.37</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>49.26</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>49.26</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>49.26</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>GREAT BRITAIN</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Great Britain Pound</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>GBP</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>57.24</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>57.1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>56.683</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>58.95</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>58.95</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>58.95</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>HONG KONG</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Hong Kong Dollar</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>HKD</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>5.89</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>5.73</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>6.23</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>6.23</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>INDIA</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>India Rupee</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>INR</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0.5347</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0.5689</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0.5689</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>JAPAN</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Japan Yen</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>JPY</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>30.81</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>30.04</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>32.44</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>32.44</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>KENYA</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Kenya Shilling</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>KES</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>36.57</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>38.11</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>MADAGASCAR</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Malagasy Ariary</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>MGA</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1.01</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1.07</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>NEW ZEALAND</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Cook Islands New Zealand Dollars</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>NZD</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>26.16</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>25.7</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>27.39</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>27.39</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>NORWAY</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Bouvet Island Norway Kroner</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>NOK</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>4.05</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>3.93</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>4.28</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>4.28</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>PAKISTAN</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Pakistan Rupees</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>PKR</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>16.5</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>17.47</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>SAUDI ARABIA</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Saudi Arabia Riyals</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>SAR</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>12.28</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>11.97</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>12.99</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>12.99</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>SEYCHELLES</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Seychelles Rupees</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>SCR</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>3.17</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>2.92</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>3.47</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>3.47</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>SINGAPORE</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Singapore Dollars</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>SGD</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>33.84</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>33.59</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>35.63</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>35.63</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>SOUTH AFRICA</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>South Africa Rand</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>ZAR</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>2.52</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>2.47</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>2.68</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>2.68</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>SRI LANKA</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Sri Lanka Rupee</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>LKR</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>15.84</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>16.58</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>SWEDEN</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Sweden Kronor</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>SEK</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>4.18</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>4.06</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>4.38</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>4.38</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>SWITZERLAND</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Switzerland Franc</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>CHF</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>51.09</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>50.58</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>53.8</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>53.8</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>TANZANIA</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>Tanzania Shillings</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>TZS</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1.81</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1.9</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>UNITED ARAB EMIRATES</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>UAE Dirham</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>AED</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>12.86</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>11.91</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>13.46</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>13.46</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="str">
+        <x:v>USA</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>United States Dollars</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>USD</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>46.29</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>46.09</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>47.19</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>47.19</x:v>
+      </x:c>
+      <x:c s="1" t="n">
+        <x:v>47.662</x:v>
+      </x:c>
+      <x:c s="1" t="str">
+        <x:v>07-Feb-2025 08:56</x:v>
+      </x:c>
+    </x:row>
     <x:row/>
     <x:row>
       <x:c s="2" t="str">

</xml_diff>